<commit_message>
Created a functioning version of Janbu_corrected. Got right of MP versions. This should be the final set of solution methods for now.
</commit_message>
<xml_diff>
--- a/docs/input_template.xlsx
+++ b/docs/input_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8543402D-81BD-D540-8CA7-368B8E7A5FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8756A91-1044-244C-B164-8B1325D7E593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="1220" windowWidth="32160" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2880" yWindow="2740" windowWidth="32160" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="crack_depth">main!$D$17</definedName>
     <definedName name="crack_depth_water">main!$D$18</definedName>
     <definedName name="gamma_w">main!$D$16</definedName>
+    <definedName name="k">main!$D$19</definedName>
     <definedName name="max_depth">circles!$C$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="110">
   <si>
     <t>X</t>
   </si>
@@ -464,6 +465,9 @@
       </rPr>
       <t>(c/p)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic coefficient (k): </t>
   </si>
 </sst>
 </file>
@@ -4372,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4529,6 +4533,12 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
+      <c r="C19" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -4556,7 +4566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CEDAD3-D805-AE4D-9F0D-9E80BF51FF21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
made file i/o more robust
</commit_message>
<xml_diff>
--- a/docs/input_template.xlsx
+++ b/docs/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8756A91-1044-244C-B164-8B1325D7E593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903CC8BB-5950-D847-A8E4-A3BA730239C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2740" windowWidth="32160" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2880" yWindow="2740" windowWidth="32160" windowHeight="24340" activeTab="5" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -4376,7 +4376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5100,16 +5100,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5575,10 +5575,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6F868-4227-8740-A8A1-4745562882FC}">
-  <dimension ref="A2:K14"/>
+  <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5773,6 +5773,12 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
+    </row>
+    <row r="18" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5789,7 +5795,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added logic for tension cracks.
</commit_message>
<xml_diff>
--- a/docs/input_template.xlsx
+++ b/docs/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903CC8BB-5950-D847-A8E4-A3BA730239C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFEBB88-6075-2D4D-999D-BBCF485D3789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2740" windowWidth="32160" windowHeight="24340" activeTab="5" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2880" yWindow="2740" windowWidth="32160" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -4376,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4520,7 +4520,7 @@
         <v>80</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -5577,7 +5577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6F868-4227-8740-A8A1-4745562882FC}">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>